<commit_message>
Eurostat Editorial Content update
</commit_message>
<xml_diff>
--- a/KD model/NLP4StatRef-SE-Article-Mapping.xlsx
+++ b/KD model/NLP4StatRef-SE-Article-Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pro\LuapLab\Prestations\Union Européenne\Eurostat\KnowledgeDatabase\Mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3E5A04-0431-4FC7-8C70-F2E304534478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848D527C-3C58-432B-B106-BF50725C13FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10536" firstSheet="3" activeTab="3" xr2:uid="{1A192BEA-C8B5-4BCA-8CD2-9EE6E1FF3F35}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10536" firstSheet="2" activeTab="2" xr2:uid="{1A192BEA-C8B5-4BCA-8CD2-9EE6E1FF3F35}"/>
   </bookViews>
   <sheets>
     <sheet name="HistoVersion" sheetId="4" r:id="rId1"/>
@@ -21,10 +21,10 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'CD-SE-Article'!$A$1:$K$60</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'KD-SE-Article'!$A$1:$N$57</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'KD-SE-Article-CoreData'!$A$1:$N$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'KD-SE-Article'!$A$1:$N$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'KD-SE-Article-CoreData'!$A$1:$N$27</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="214">
   <si>
     <t>workDate</t>
   </si>
@@ -562,12 +562,6 @@
     <t>2021.04.02 - EP : at this stage, this property couldn't be instanciate. Waiting for the linking with Dcat.</t>
   </si>
   <si>
-    <t>excel\id ?</t>
-  </si>
-  <si>
-    <t>estat:StatisticsExplainedData</t>
-  </si>
-  <si>
     <t>estat:relatedStatisticData</t>
   </si>
   <si>
@@ -576,12 +570,6 @@
   </si>
   <si>
     <t>estat:sourceData</t>
-  </si>
-  <si>
-    <t>estat:StatisticsExplainedData @rdf:about</t>
-  </si>
-  <si>
-    <t>https://nlp4statref/knowledge/resource/statistics-explained-data#SeqNum</t>
   </si>
   <si>
     <t>SE Article
@@ -845,6 +833,95 @@
   </si>
   <si>
     <t>Suppress the words "Statistical article".</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Lao UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>2021.08.16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Lao UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - EP : new property to differentiate SE and Experimental Statistics</t>
+    </r>
+  </si>
+  <si>
+    <t>dct:description</t>
+  </si>
+  <si>
+    <t>Statistics Explained article</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>KD Update
+- New property : dct:description
+- Rename StatisticsExplainedData =&gt; StatisticalDataReport</t>
+  </si>
+  <si>
+    <t>estat:StatisticalDataReport</t>
+  </si>
+  <si>
+    <t>estat:estat:StatisticalDataReport @rdf:about</t>
+  </si>
+  <si>
+    <t>https://nlp4statref/knowledge/resource/statistical-data-report#SeqNum</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Lao UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>2021.08.16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Lao UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - EP : rename class and URI change</t>
+    </r>
+  </si>
+  <si>
+    <t>excel\id</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Lao UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>2021.08.16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Lao UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - EP : Rename StatisticsExplainedData =&gt; StatisticalDataReport</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1259,7 +1336,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1578,39 +1655,81 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1652,30 +1771,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2077,7 +2172,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.7" x14ac:dyDescent="0.65"/>
@@ -2134,13 +2229,13 @@
         <v>44392</v>
       </c>
       <c r="B4" s="85" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C4" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="D4" s="137" t="s">
-        <v>182</v>
+      <c r="D4" s="114" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="44.1" x14ac:dyDescent="0.65">
@@ -2148,20 +2243,28 @@
         <v>44399</v>
       </c>
       <c r="B5" s="85" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C5" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="D5" s="137" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.65">
-      <c r="A6" s="87"/>
-      <c r="B6" s="85"/>
-      <c r="C6" s="85"/>
-      <c r="D6" s="88"/>
+      <c r="D5" s="114" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="44.1" x14ac:dyDescent="0.65">
+      <c r="A6" s="92">
+        <v>44426</v>
+      </c>
+      <c r="B6" s="85" t="s">
+        <v>206</v>
+      </c>
+      <c r="C6" s="85" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="114" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A7" s="87"/>
@@ -2268,7 +2371,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38E39D9-7E53-411A-904C-D894E3105FE5}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.7" x14ac:dyDescent="0.65"/>
   <cols>
@@ -2353,13 +2458,13 @@
       <c r="D3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="118" t="s">
+      <c r="E3" s="126" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="132" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="116">
+      <c r="G3" s="127">
         <v>1</v>
       </c>
       <c r="H3" s="11" t="s">
@@ -2377,21 +2482,21 @@
         <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="118"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="116"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="133"/>
+      <c r="G4" s="127"/>
       <c r="H4" s="11" t="s">
         <v>78</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="11"/>
       <c r="K4" s="20" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="132.30000000000001" x14ac:dyDescent="0.65">
@@ -2402,21 +2507,21 @@
         <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="118"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="116"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="127"/>
       <c r="H5" s="11" t="s">
         <v>80</v>
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="11"/>
       <c r="K5" s="20" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.65">
@@ -2516,23 +2621,23 @@
       <c r="C9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="117" t="s">
+      <c r="D9" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="118" t="s">
+      <c r="E9" s="126" t="s">
         <v>27</v>
       </c>
       <c r="F9" s="11"/>
-      <c r="G9" s="116" t="s">
+      <c r="G9" s="127" t="s">
         <v>28</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="122" t="s">
+      <c r="J9" s="135" t="s">
         <v>29</v>
       </c>
-      <c r="K9" s="114" t="s">
-        <v>202</v>
+      <c r="K9" s="113" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="55.8" customHeight="1" x14ac:dyDescent="0.65">
@@ -2543,18 +2648,18 @@
         <v>11</v>
       </c>
       <c r="C10" s="12"/>
-      <c r="D10" s="117"/>
-      <c r="E10" s="118"/>
+      <c r="D10" s="125"/>
+      <c r="E10" s="126"/>
       <c r="F10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="116"/>
+      <c r="G10" s="127"/>
       <c r="H10" s="11" t="s">
         <v>30</v>
       </c>
       <c r="I10" s="11"/>
-      <c r="J10" s="144"/>
-      <c r="K10" s="114"/>
+      <c r="J10" s="136"/>
+      <c r="K10" s="113"/>
     </row>
     <row r="11" spans="1:11" ht="55.8" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A11" s="3">
@@ -2564,18 +2669,18 @@
         <v>11</v>
       </c>
       <c r="C11" s="12"/>
-      <c r="D11" s="117"/>
-      <c r="E11" s="118"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="126"/>
       <c r="F11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="116"/>
+      <c r="G11" s="127"/>
       <c r="H11" s="11" t="s">
         <v>31</v>
       </c>
       <c r="I11" s="11"/>
-      <c r="J11" s="144"/>
-      <c r="K11" s="114"/>
+      <c r="J11" s="136"/>
+      <c r="K11" s="113"/>
     </row>
     <row r="12" spans="1:11" ht="58.8" x14ac:dyDescent="0.65">
       <c r="A12" s="3">
@@ -2585,21 +2690,21 @@
         <v>11</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D12" s="117"/>
-      <c r="E12" s="118"/>
+        <v>200</v>
+      </c>
+      <c r="D12" s="125"/>
+      <c r="E12" s="126"/>
       <c r="F12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="116"/>
+      <c r="G12" s="127"/>
       <c r="H12" s="102" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="I12" s="20"/>
-      <c r="J12" s="144"/>
-      <c r="K12" s="114" t="s">
-        <v>184</v>
+      <c r="J12" s="136"/>
+      <c r="K12" s="113" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="58.8" x14ac:dyDescent="0.65">
@@ -2610,21 +2715,21 @@
         <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D13" s="117"/>
-      <c r="E13" s="118"/>
+        <v>200</v>
+      </c>
+      <c r="D13" s="125"/>
+      <c r="E13" s="126"/>
       <c r="F13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="116"/>
+      <c r="G13" s="127"/>
       <c r="H13" s="102" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="I13" s="20"/>
-      <c r="J13" s="123"/>
-      <c r="K13" s="114" t="s">
-        <v>203</v>
+      <c r="J13" s="137"/>
+      <c r="K13" s="113" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="58.8" x14ac:dyDescent="0.65">
@@ -2654,7 +2759,7 @@
       <c r="J14" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="114"/>
+      <c r="K14" s="113"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A15" s="3">
@@ -2691,14 +2796,14 @@
         <v>11</v>
       </c>
       <c r="C16" s="12"/>
-      <c r="D16" s="117" t="s">
+      <c r="D16" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="118" t="s">
+      <c r="E16" s="126" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="116" t="s">
+      <c r="F16" s="7"/>
+      <c r="G16" s="127" t="s">
         <v>58</v>
       </c>
       <c r="H16" s="11" t="s">
@@ -2718,12 +2823,12 @@
         <v>11</v>
       </c>
       <c r="C17" s="12"/>
-      <c r="D17" s="117"/>
-      <c r="E17" s="118"/>
+      <c r="D17" s="125"/>
+      <c r="E17" s="126"/>
       <c r="F17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="116"/>
+      <c r="G17" s="127"/>
       <c r="H17" s="11" t="s">
         <v>39</v>
       </c>
@@ -2739,12 +2844,12 @@
         <v>11</v>
       </c>
       <c r="C18" s="12"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="118"/>
-      <c r="F18" s="115" t="s">
+      <c r="D18" s="125"/>
+      <c r="E18" s="126"/>
+      <c r="F18" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="116"/>
+      <c r="G18" s="127"/>
       <c r="H18" s="11" t="s">
         <v>40</v>
       </c>
@@ -2760,10 +2865,10 @@
         <v>11</v>
       </c>
       <c r="C19" s="5"/>
-      <c r="D19" s="117"/>
-      <c r="E19" s="118"/>
-      <c r="F19" s="115"/>
-      <c r="G19" s="116"/>
+      <c r="D19" s="125"/>
+      <c r="E19" s="126"/>
+      <c r="F19" s="130"/>
+      <c r="G19" s="127"/>
       <c r="H19" s="11" t="s">
         <v>85</v>
       </c>
@@ -2783,10 +2888,10 @@
         <v>11</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="117"/>
-      <c r="E20" s="118"/>
-      <c r="F20" s="115"/>
-      <c r="G20" s="116"/>
+      <c r="D20" s="125"/>
+      <c r="E20" s="126"/>
+      <c r="F20" s="130"/>
+      <c r="G20" s="127"/>
       <c r="H20" s="11" t="s">
         <v>86</v>
       </c>
@@ -2806,14 +2911,14 @@
         <v>11</v>
       </c>
       <c r="C21" s="12"/>
-      <c r="D21" s="117" t="s">
+      <c r="D21" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="118" t="s">
+      <c r="E21" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="116" t="s">
+      <c r="F21" s="7"/>
+      <c r="G21" s="127" t="s">
         <v>87</v>
       </c>
       <c r="H21" s="11" t="s">
@@ -2833,12 +2938,12 @@
         <v>11</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="117"/>
-      <c r="E22" s="118"/>
+      <c r="D22" s="125"/>
+      <c r="E22" s="126"/>
       <c r="F22" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="116"/>
+      <c r="G22" s="127"/>
       <c r="H22" s="11" t="s">
         <v>43</v>
       </c>
@@ -2854,12 +2959,12 @@
         <v>11</v>
       </c>
       <c r="C23" s="12"/>
-      <c r="D23" s="117"/>
-      <c r="E23" s="118"/>
-      <c r="F23" s="115" t="s">
+      <c r="D23" s="125"/>
+      <c r="E23" s="126"/>
+      <c r="F23" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="116"/>
+      <c r="G23" s="127"/>
       <c r="H23" s="11" t="s">
         <v>44</v>
       </c>
@@ -2875,10 +2980,10 @@
         <v>11</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="117"/>
-      <c r="E24" s="118"/>
-      <c r="F24" s="115"/>
-      <c r="G24" s="116"/>
+      <c r="D24" s="125"/>
+      <c r="E24" s="126"/>
+      <c r="F24" s="130"/>
+      <c r="G24" s="127"/>
       <c r="H24" s="11" t="s">
         <v>88</v>
       </c>
@@ -2898,10 +3003,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="117"/>
-      <c r="E25" s="118"/>
-      <c r="F25" s="115"/>
-      <c r="G25" s="116"/>
+      <c r="D25" s="125"/>
+      <c r="E25" s="126"/>
+      <c r="F25" s="130"/>
+      <c r="G25" s="127"/>
       <c r="H25" s="11" t="s">
         <v>89</v>
       </c>
@@ -2913,7 +3018,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="14.7" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="26" spans="1:11" ht="44.1" x14ac:dyDescent="0.65">
       <c r="A26" s="3">
         <v>44351</v>
       </c>
@@ -2921,14 +3026,14 @@
         <v>11</v>
       </c>
       <c r="C26" s="12"/>
-      <c r="D26" s="117" t="s">
+      <c r="D26" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="118" t="s">
+      <c r="E26" s="126" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="116" t="s">
+      <c r="F26" s="7"/>
+      <c r="G26" s="127" t="s">
         <v>58</v>
       </c>
       <c r="H26" s="11" t="s">
@@ -2948,12 +3053,12 @@
         <v>11</v>
       </c>
       <c r="C27" s="12"/>
-      <c r="D27" s="117"/>
-      <c r="E27" s="118"/>
+      <c r="D27" s="125"/>
+      <c r="E27" s="126"/>
       <c r="F27" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G27" s="116"/>
+      <c r="G27" s="127"/>
       <c r="H27" s="11" t="s">
         <v>47</v>
       </c>
@@ -2969,12 +3074,12 @@
         <v>11</v>
       </c>
       <c r="C28" s="12"/>
-      <c r="D28" s="117"/>
-      <c r="E28" s="118"/>
-      <c r="F28" s="115" t="s">
+      <c r="D28" s="125"/>
+      <c r="E28" s="126"/>
+      <c r="F28" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="G28" s="116"/>
+      <c r="G28" s="127"/>
       <c r="H28" s="11" t="s">
         <v>48</v>
       </c>
@@ -2990,10 +3095,10 @@
         <v>11</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="117"/>
-      <c r="E29" s="118"/>
-      <c r="F29" s="115"/>
-      <c r="G29" s="116"/>
+      <c r="D29" s="125"/>
+      <c r="E29" s="126"/>
+      <c r="F29" s="130"/>
+      <c r="G29" s="127"/>
       <c r="H29" s="11" t="s">
         <v>90</v>
       </c>
@@ -3013,10 +3118,10 @@
         <v>11</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="117"/>
-      <c r="E30" s="118"/>
-      <c r="F30" s="115"/>
-      <c r="G30" s="116"/>
+      <c r="D30" s="125"/>
+      <c r="E30" s="126"/>
+      <c r="F30" s="130"/>
+      <c r="G30" s="127"/>
       <c r="H30" s="11" t="s">
         <v>91</v>
       </c>
@@ -3036,14 +3141,14 @@
         <v>11</v>
       </c>
       <c r="C31" s="12"/>
-      <c r="D31" s="117" t="s">
+      <c r="D31" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="118" t="s">
+      <c r="E31" s="126" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="11"/>
-      <c r="G31" s="116" t="s">
+      <c r="F31" s="7"/>
+      <c r="G31" s="127" t="s">
         <v>58</v>
       </c>
       <c r="H31" s="11" t="s">
@@ -3063,12 +3168,12 @@
         <v>11</v>
       </c>
       <c r="C32" s="12"/>
-      <c r="D32" s="117"/>
-      <c r="E32" s="118"/>
+      <c r="D32" s="125"/>
+      <c r="E32" s="126"/>
       <c r="F32" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G32" s="116"/>
+      <c r="G32" s="127"/>
       <c r="H32" s="11" t="s">
         <v>51</v>
       </c>
@@ -3084,12 +3189,12 @@
         <v>11</v>
       </c>
       <c r="C33" s="12"/>
-      <c r="D33" s="117"/>
-      <c r="E33" s="118"/>
-      <c r="F33" s="115" t="s">
+      <c r="D33" s="125"/>
+      <c r="E33" s="126"/>
+      <c r="F33" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="G33" s="116"/>
+      <c r="G33" s="127"/>
       <c r="H33" s="11" t="s">
         <v>52</v>
       </c>
@@ -3105,10 +3210,10 @@
         <v>11</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="117"/>
-      <c r="E34" s="118"/>
-      <c r="F34" s="115"/>
-      <c r="G34" s="116"/>
+      <c r="D34" s="125"/>
+      <c r="E34" s="126"/>
+      <c r="F34" s="130"/>
+      <c r="G34" s="127"/>
       <c r="H34" s="11" t="s">
         <v>92</v>
       </c>
@@ -3128,10 +3233,10 @@
         <v>11</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="D35" s="117"/>
-      <c r="E35" s="118"/>
-      <c r="F35" s="115"/>
-      <c r="G35" s="116"/>
+      <c r="D35" s="125"/>
+      <c r="E35" s="126"/>
+      <c r="F35" s="130"/>
+      <c r="G35" s="127"/>
       <c r="H35" s="11" t="s">
         <v>93</v>
       </c>
@@ -3151,14 +3256,14 @@
         <v>11</v>
       </c>
       <c r="C36" s="12"/>
-      <c r="D36" s="117" t="s">
+      <c r="D36" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="118" t="s">
+      <c r="E36" s="126" t="s">
         <v>53</v>
       </c>
-      <c r="F36" s="11"/>
-      <c r="G36" s="116" t="s">
+      <c r="F36" s="7"/>
+      <c r="G36" s="127" t="s">
         <v>58</v>
       </c>
       <c r="H36" s="11" t="s">
@@ -3178,12 +3283,12 @@
         <v>11</v>
       </c>
       <c r="C37" s="12"/>
-      <c r="D37" s="117"/>
-      <c r="E37" s="118"/>
+      <c r="D37" s="125"/>
+      <c r="E37" s="126"/>
       <c r="F37" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G37" s="116"/>
+      <c r="G37" s="127"/>
       <c r="H37" s="11" t="s">
         <v>55</v>
       </c>
@@ -3199,12 +3304,12 @@
         <v>11</v>
       </c>
       <c r="C38" s="12"/>
-      <c r="D38" s="117"/>
-      <c r="E38" s="118"/>
-      <c r="F38" s="115" t="s">
+      <c r="D38" s="125"/>
+      <c r="E38" s="126"/>
+      <c r="F38" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="G38" s="116"/>
+      <c r="G38" s="127"/>
       <c r="H38" s="11" t="s">
         <v>56</v>
       </c>
@@ -3220,10 +3325,10 @@
         <v>11</v>
       </c>
       <c r="C39" s="5"/>
-      <c r="D39" s="117"/>
-      <c r="E39" s="118"/>
-      <c r="F39" s="115"/>
-      <c r="G39" s="116"/>
+      <c r="D39" s="125"/>
+      <c r="E39" s="126"/>
+      <c r="F39" s="130"/>
+      <c r="G39" s="127"/>
       <c r="H39" s="11" t="s">
         <v>94</v>
       </c>
@@ -3243,10 +3348,10 @@
         <v>11</v>
       </c>
       <c r="C40" s="5"/>
-      <c r="D40" s="117"/>
-      <c r="E40" s="118"/>
-      <c r="F40" s="115"/>
-      <c r="G40" s="116"/>
+      <c r="D40" s="125"/>
+      <c r="E40" s="126"/>
+      <c r="F40" s="130"/>
+      <c r="G40" s="127"/>
       <c r="H40" s="11" t="s">
         <v>95</v>
       </c>
@@ -3266,14 +3371,14 @@
         <v>11</v>
       </c>
       <c r="C41" s="12"/>
-      <c r="D41" s="117" t="s">
+      <c r="D41" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="E41" s="118" t="s">
+      <c r="E41" s="126" t="s">
         <v>57</v>
       </c>
-      <c r="F41" s="11"/>
-      <c r="G41" s="116" t="s">
+      <c r="F41" s="7"/>
+      <c r="G41" s="127" t="s">
         <v>58</v>
       </c>
       <c r="H41" s="11" t="s">
@@ -3293,12 +3398,12 @@
         <v>11</v>
       </c>
       <c r="C42" s="12"/>
-      <c r="D42" s="117"/>
-      <c r="E42" s="118"/>
+      <c r="D42" s="125"/>
+      <c r="E42" s="126"/>
       <c r="F42" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G42" s="116"/>
+      <c r="G42" s="127"/>
       <c r="H42" s="11" t="s">
         <v>60</v>
       </c>
@@ -3314,12 +3419,12 @@
         <v>11</v>
       </c>
       <c r="C43" s="12"/>
-      <c r="D43" s="117"/>
-      <c r="E43" s="118"/>
-      <c r="F43" s="115" t="s">
+      <c r="D43" s="125"/>
+      <c r="E43" s="126"/>
+      <c r="F43" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="G43" s="116"/>
+      <c r="G43" s="127"/>
       <c r="H43" s="11" t="s">
         <v>61</v>
       </c>
@@ -3335,10 +3440,10 @@
         <v>11</v>
       </c>
       <c r="C44" s="5"/>
-      <c r="D44" s="117"/>
-      <c r="E44" s="118"/>
-      <c r="F44" s="115"/>
-      <c r="G44" s="116"/>
+      <c r="D44" s="125"/>
+      <c r="E44" s="126"/>
+      <c r="F44" s="130"/>
+      <c r="G44" s="127"/>
       <c r="H44" s="11" t="s">
         <v>96</v>
       </c>
@@ -3358,10 +3463,10 @@
         <v>11</v>
       </c>
       <c r="C45" s="5"/>
-      <c r="D45" s="117"/>
-      <c r="E45" s="118"/>
-      <c r="F45" s="115"/>
-      <c r="G45" s="116"/>
+      <c r="D45" s="125"/>
+      <c r="E45" s="126"/>
+      <c r="F45" s="130"/>
+      <c r="G45" s="127"/>
       <c r="H45" s="11" t="s">
         <v>97</v>
       </c>
@@ -3381,14 +3486,14 @@
         <v>11</v>
       </c>
       <c r="C46" s="12"/>
-      <c r="D46" s="117" t="s">
+      <c r="D46" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="E46" s="118" t="s">
+      <c r="E46" s="126" t="s">
         <v>62</v>
       </c>
-      <c r="F46" s="11"/>
-      <c r="G46" s="116" t="s">
+      <c r="F46" s="7"/>
+      <c r="G46" s="127" t="s">
         <v>58</v>
       </c>
       <c r="H46" s="11" t="s">
@@ -3408,12 +3513,12 @@
         <v>11</v>
       </c>
       <c r="C47" s="12"/>
-      <c r="D47" s="117"/>
-      <c r="E47" s="118"/>
+      <c r="D47" s="125"/>
+      <c r="E47" s="126"/>
       <c r="F47" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G47" s="116"/>
+      <c r="G47" s="127"/>
       <c r="H47" s="11" t="s">
         <v>64</v>
       </c>
@@ -3429,12 +3534,12 @@
         <v>11</v>
       </c>
       <c r="C48" s="12"/>
-      <c r="D48" s="117"/>
-      <c r="E48" s="118"/>
-      <c r="F48" s="115" t="s">
+      <c r="D48" s="125"/>
+      <c r="E48" s="126"/>
+      <c r="F48" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="G48" s="116"/>
+      <c r="G48" s="127"/>
       <c r="H48" s="11" t="s">
         <v>65</v>
       </c>
@@ -3450,10 +3555,10 @@
         <v>11</v>
       </c>
       <c r="C49" s="5"/>
-      <c r="D49" s="117"/>
-      <c r="E49" s="118"/>
-      <c r="F49" s="115"/>
-      <c r="G49" s="116"/>
+      <c r="D49" s="125"/>
+      <c r="E49" s="126"/>
+      <c r="F49" s="130"/>
+      <c r="G49" s="127"/>
       <c r="H49" s="11" t="s">
         <v>98</v>
       </c>
@@ -3473,10 +3578,10 @@
         <v>11</v>
       </c>
       <c r="C50" s="5"/>
-      <c r="D50" s="117"/>
-      <c r="E50" s="118"/>
-      <c r="F50" s="115"/>
-      <c r="G50" s="116"/>
+      <c r="D50" s="125"/>
+      <c r="E50" s="126"/>
+      <c r="F50" s="130"/>
+      <c r="G50" s="127"/>
       <c r="H50" s="11" t="s">
         <v>99</v>
       </c>
@@ -3496,14 +3601,14 @@
         <v>11</v>
       </c>
       <c r="C51" s="12"/>
-      <c r="D51" s="117" t="s">
+      <c r="D51" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="E51" s="118" t="s">
+      <c r="E51" s="126" t="s">
         <v>66</v>
       </c>
-      <c r="F51" s="11"/>
-      <c r="G51" s="116" t="s">
+      <c r="F51" s="7"/>
+      <c r="G51" s="127" t="s">
         <v>58</v>
       </c>
       <c r="H51" s="11" t="s">
@@ -3523,12 +3628,12 @@
         <v>11</v>
       </c>
       <c r="C52" s="12"/>
-      <c r="D52" s="117"/>
-      <c r="E52" s="118"/>
+      <c r="D52" s="125"/>
+      <c r="E52" s="126"/>
       <c r="F52" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G52" s="116"/>
+      <c r="G52" s="127"/>
       <c r="H52" s="11" t="s">
         <v>68</v>
       </c>
@@ -3544,12 +3649,12 @@
         <v>11</v>
       </c>
       <c r="C53" s="12"/>
-      <c r="D53" s="117"/>
-      <c r="E53" s="118"/>
-      <c r="F53" s="115" t="s">
+      <c r="D53" s="125"/>
+      <c r="E53" s="126"/>
+      <c r="F53" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="G53" s="116"/>
+      <c r="G53" s="127"/>
       <c r="H53" s="11" t="s">
         <v>69</v>
       </c>
@@ -3565,10 +3670,10 @@
         <v>11</v>
       </c>
       <c r="C54" s="5"/>
-      <c r="D54" s="117"/>
-      <c r="E54" s="118"/>
-      <c r="F54" s="115"/>
-      <c r="G54" s="116"/>
+      <c r="D54" s="125"/>
+      <c r="E54" s="126"/>
+      <c r="F54" s="130"/>
+      <c r="G54" s="127"/>
       <c r="H54" s="11" t="s">
         <v>100</v>
       </c>
@@ -3588,10 +3693,10 @@
         <v>11</v>
       </c>
       <c r="C55" s="5"/>
-      <c r="D55" s="117"/>
-      <c r="E55" s="118"/>
-      <c r="F55" s="115"/>
-      <c r="G55" s="116"/>
+      <c r="D55" s="125"/>
+      <c r="E55" s="126"/>
+      <c r="F55" s="130"/>
+      <c r="G55" s="127"/>
       <c r="H55" s="11" t="s">
         <v>101</v>
       </c>
@@ -3613,14 +3718,14 @@
       <c r="C56" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D56" s="117" t="s">
+      <c r="D56" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="E56" s="120" t="s">
+      <c r="E56" s="128" t="s">
         <v>71</v>
       </c>
       <c r="F56" s="14"/>
-      <c r="G56" s="121" t="s">
+      <c r="G56" s="129" t="s">
         <v>58</v>
       </c>
       <c r="H56" s="14" t="s">
@@ -3628,7 +3733,7 @@
       </c>
       <c r="I56" s="14"/>
       <c r="J56" s="14"/>
-      <c r="K56" s="119" t="s">
+      <c r="K56" s="131" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3640,18 +3745,18 @@
         <v>70</v>
       </c>
       <c r="C57" s="12"/>
-      <c r="D57" s="117"/>
-      <c r="E57" s="120"/>
+      <c r="D57" s="125"/>
+      <c r="E57" s="128"/>
       <c r="F57" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G57" s="121"/>
+      <c r="G57" s="129"/>
       <c r="H57" s="14" t="s">
         <v>73</v>
       </c>
       <c r="I57" s="14"/>
       <c r="J57" s="14"/>
-      <c r="K57" s="119"/>
+      <c r="K57" s="131"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A58" s="3">
@@ -3661,18 +3766,18 @@
         <v>70</v>
       </c>
       <c r="C58" s="12"/>
-      <c r="D58" s="117"/>
-      <c r="E58" s="120"/>
+      <c r="D58" s="125"/>
+      <c r="E58" s="128"/>
       <c r="F58" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G58" s="121"/>
+      <c r="G58" s="129"/>
       <c r="H58" s="14" t="s">
         <v>74</v>
       </c>
       <c r="I58" s="14"/>
       <c r="J58" s="14"/>
-      <c r="K58" s="119"/>
+      <c r="K58" s="131"/>
     </row>
     <row r="59" spans="1:11" ht="117.6" x14ac:dyDescent="0.65">
       <c r="A59" s="3">
@@ -3682,31 +3787,31 @@
         <v>70</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="D59" s="138" t="s">
+        <v>185</v>
+      </c>
+      <c r="D59" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="E59" s="139" t="s">
+      <c r="E59" s="116" t="s">
         <v>75</v>
       </c>
-      <c r="F59" s="140" t="s">
+      <c r="F59" s="117" t="s">
         <v>18</v>
       </c>
-      <c r="G59" s="141" t="s">
+      <c r="G59" s="118" t="s">
         <v>28</v>
       </c>
       <c r="H59" s="14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="I59" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="J59" s="10" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="K59" s="20" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.65">
@@ -3751,7 +3856,16 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K60" xr:uid="{E201601C-0217-4F72-B294-396D8744DE8C}"/>
-  <mergeCells count="42">
+  <mergeCells count="43">
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="G16:G20"/>
+    <mergeCell ref="K56:K58"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="G21:G25"/>
+    <mergeCell ref="F3:F5"/>
     <mergeCell ref="J9:J13"/>
     <mergeCell ref="G31:G35"/>
     <mergeCell ref="G36:G40"/>
@@ -3759,12 +3873,6 @@
     <mergeCell ref="F38:F40"/>
     <mergeCell ref="F28:F30"/>
     <mergeCell ref="F33:F35"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="G16:G20"/>
-    <mergeCell ref="K56:K58"/>
-    <mergeCell ref="F53:F55"/>
     <mergeCell ref="D41:D45"/>
     <mergeCell ref="E41:E45"/>
     <mergeCell ref="G41:G45"/>
@@ -3787,8 +3895,6 @@
     <mergeCell ref="E21:E25"/>
     <mergeCell ref="D26:D30"/>
     <mergeCell ref="E26:E30"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="G21:G25"/>
     <mergeCell ref="D9:D13"/>
     <mergeCell ref="E9:E13"/>
     <mergeCell ref="G9:G13"/>
@@ -3814,13 +3920,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC1E54C3-F8CA-4360-B13A-23EFE6E31915}">
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="5574" ySplit="480" topLeftCell="F1" activePane="bottomRight"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="5574" ySplit="480" topLeftCell="D19" activePane="bottomLeft"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
-      <selection pane="bottomRight" activeCell="E46" sqref="E46"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.7" x14ac:dyDescent="0.65"/>
@@ -4105,7 +4211,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="27"/>
@@ -4118,8 +4224,8 @@
         <v>115</v>
       </c>
       <c r="L10" s="29"/>
-      <c r="M10" s="142" t="s">
-        <v>190</v>
+      <c r="M10" s="119" t="s">
+        <v>186</v>
       </c>
       <c r="N10" s="32"/>
       <c r="O10" s="100"/>
@@ -4132,7 +4238,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="45" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="34"/>
@@ -4145,8 +4251,8 @@
         <v>115</v>
       </c>
       <c r="L11" s="29"/>
-      <c r="M11" s="142" t="s">
-        <v>191</v>
+      <c r="M11" s="119" t="s">
+        <v>187</v>
       </c>
       <c r="N11" s="32"/>
       <c r="O11" s="99"/>
@@ -4193,7 +4299,7 @@
         <v>115</v>
       </c>
       <c r="L13" s="38" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="M13" s="31"/>
       <c r="N13" s="56" t="s">
@@ -4242,7 +4348,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="45" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D15" s="48" t="s">
         <v>12</v>
@@ -4265,11 +4371,11 @@
         <v>115</v>
       </c>
       <c r="L15" s="38" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="M15" s="38"/>
       <c r="N15" s="101" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="O15" s="99"/>
     </row>
@@ -4284,12 +4390,12 @@
       <c r="D16" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="112" t="s">
+      <c r="E16" s="121" t="s">
         <v>19</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="52"/>
-      <c r="H16" s="113" t="s">
+      <c r="H16" s="122" t="s">
         <v>128</v>
       </c>
       <c r="I16" s="54" t="s">
@@ -4298,7 +4404,7 @@
       <c r="J16" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="K16" s="113" t="s">
+      <c r="K16" s="122" t="s">
         <v>115</v>
       </c>
       <c r="L16" s="53"/>
@@ -4306,110 +4412,114 @@
       <c r="N16" s="32"/>
       <c r="O16" s="99"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:15" ht="58.8" x14ac:dyDescent="0.65">
       <c r="A17" s="26">
-        <v>44392</v>
+        <v>44424</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="45"/>
+      <c r="C17" s="45" t="s">
+        <v>203</v>
+      </c>
       <c r="D17" s="48" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="35"/>
       <c r="G17" s="52"/>
-      <c r="H17" s="113" t="s">
+      <c r="H17" s="112" t="s">
         <v>128</v>
       </c>
       <c r="I17" s="54" t="s">
-        <v>179</v>
-      </c>
-      <c r="J17" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="K17" s="113" t="s">
+        <v>204</v>
+      </c>
+      <c r="J17" s="53" t="s">
+        <v>132</v>
+      </c>
+      <c r="K17" s="112" t="s">
         <v>115</v>
       </c>
-      <c r="L17" s="38" t="s">
-        <v>180</v>
+      <c r="L17" s="123" t="s">
+        <v>205</v>
       </c>
       <c r="M17" s="31"/>
-      <c r="N17" s="101" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="29.4" x14ac:dyDescent="0.65">
+      <c r="N17" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="O17" s="99"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.65">
       <c r="A18" s="26">
-        <v>44399</v>
+        <v>44392</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="45" t="s">
-        <v>196</v>
-      </c>
+      <c r="C18" s="45"/>
       <c r="D18" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="11" t="s">
-        <v>78</v>
-      </c>
+      <c r="E18" s="27"/>
       <c r="F18" s="35"/>
       <c r="G18" s="52"/>
-      <c r="H18" s="50" t="s">
+      <c r="H18" s="112" t="s">
         <v>128</v>
       </c>
-      <c r="I18" s="55" t="s">
-        <v>133</v>
+      <c r="I18" s="54" t="s">
+        <v>175</v>
       </c>
       <c r="J18" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="K18" s="50" t="s">
+      <c r="K18" s="112" t="s">
         <v>115</v>
       </c>
       <c r="L18" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="M18" s="38"/>
+        <v>176</v>
+      </c>
+      <c r="M18" s="31"/>
       <c r="N18" s="101" t="s">
-        <v>195</v>
-      </c>
-      <c r="O18" s="99"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.65">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="29.4" x14ac:dyDescent="0.65">
       <c r="A19" s="26">
-        <v>44352</v>
+        <v>44399</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="45"/>
+      <c r="C19" s="45" t="s">
+        <v>192</v>
+      </c>
       <c r="D19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="31" t="s">
-        <v>138</v>
+      <c r="E19" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="F19" s="35"/>
       <c r="G19" s="52"/>
       <c r="H19" s="50" t="s">
         <v>128</v>
       </c>
-      <c r="I19" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="J19" s="58" t="s">
-        <v>135</v>
+      <c r="I19" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="J19" s="31" t="s">
+        <v>130</v>
       </c>
       <c r="K19" s="50" t="s">
         <v>115</v>
       </c>
-      <c r="L19" s="58"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="32"/>
+      <c r="L19" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="M19" s="38"/>
+      <c r="N19" s="101" t="s">
+        <v>191</v>
+      </c>
       <c r="O19" s="99"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.65">
@@ -4424,151 +4534,157 @@
         <v>12</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>16</v>
+        <v>138</v>
       </c>
       <c r="F20" s="35"/>
       <c r="G20" s="52"/>
       <c r="H20" s="50" t="s">
         <v>128</v>
       </c>
-      <c r="I20" s="54" t="s">
-        <v>136</v>
-      </c>
-      <c r="J20" s="59" t="s">
-        <v>130</v>
+      <c r="I20" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="J20" s="58" t="s">
+        <v>135</v>
       </c>
       <c r="K20" s="50" t="s">
         <v>115</v>
       </c>
-      <c r="L20" s="59"/>
+      <c r="L20" s="58"/>
       <c r="M20" s="31"/>
       <c r="N20" s="32"/>
       <c r="O20" s="99"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="A21" s="39"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
+      <c r="A21" s="26">
+        <v>44352</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="45"/>
+      <c r="D21" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>16</v>
+      </c>
       <c r="F21" s="35"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="40"/>
-      <c r="N21" s="44"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="50" t="s">
+        <v>128</v>
+      </c>
+      <c r="I21" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="J21" s="59" t="s">
+        <v>130</v>
+      </c>
+      <c r="K21" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="L21" s="59"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="32"/>
       <c r="O21" s="99"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="A22" s="26">
-        <v>44352</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="45"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="7"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
       <c r="F22" s="35"/>
-      <c r="G22" s="60" t="s">
-        <v>139</v>
-      </c>
-      <c r="H22" s="30"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="63"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="56"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="44"/>
       <c r="O22" s="99"/>
     </row>
-    <row r="23" spans="1:15" ht="102.9" x14ac:dyDescent="0.65">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.65">
       <c r="A23" s="26">
         <v>44352</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="D23" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="45"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="H23" s="30"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="99"/>
+    </row>
+    <row r="24" spans="1:15" ht="102.9" x14ac:dyDescent="0.65">
+      <c r="A24" s="26">
+        <v>44426</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="45" t="s">
+        <v>213</v>
+      </c>
+      <c r="D24" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="94"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="105" t="s">
+      <c r="E24" s="124" t="s">
+        <v>212</v>
+      </c>
+      <c r="F24" s="35"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="105" t="s">
         <v>128</v>
       </c>
-      <c r="I23" s="106" t="s">
-        <v>168</v>
-      </c>
-      <c r="J23" s="66" t="s">
-        <v>165</v>
-      </c>
-      <c r="K23" s="65" t="s">
+      <c r="I24" s="106" t="s">
+        <v>166</v>
+      </c>
+      <c r="J24" s="66" t="s">
+        <v>208</v>
+      </c>
+      <c r="K24" s="65" t="s">
         <v>115</v>
       </c>
-      <c r="L23" s="66" t="s">
+      <c r="L24" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="M23" s="67"/>
-      <c r="N23" s="68" t="s">
+      <c r="M24" s="67"/>
+      <c r="N24" s="68" t="s">
         <v>145</v>
       </c>
-      <c r="O23" s="99"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="A24" s="39"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="44"/>
       <c r="O24" s="99"/>
     </row>
-    <row r="25" spans="1:15" ht="147" x14ac:dyDescent="0.65">
-      <c r="A25" s="26">
-        <v>44352</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="45"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="7"/>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.65">
+      <c r="A25" s="39"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
       <c r="F25" s="35"/>
-      <c r="G25" s="60" t="s">
-        <v>139</v>
-      </c>
-      <c r="H25" s="30"/>
-      <c r="I25" s="62" t="s">
-        <v>140</v>
-      </c>
-      <c r="J25" s="63" t="s">
-        <v>141</v>
-      </c>
-      <c r="K25" s="30"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="56" t="s">
-        <v>142</v>
-      </c>
+      <c r="G25" s="42"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="44"/>
       <c r="O25" s="99"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.65">
+    <row r="26" spans="1:15" ht="147" x14ac:dyDescent="0.65">
       <c r="A26" s="26">
         <v>44352</v>
       </c>
@@ -4576,32 +4692,24 @@
         <v>11</v>
       </c>
       <c r="C26" s="45"/>
-      <c r="D26" s="130" t="s">
-        <v>167</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>37</v>
-      </c>
+      <c r="D26" s="46"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="35"/>
-      <c r="G26" s="135"/>
-      <c r="H26" s="136" t="s">
-        <v>128</v>
-      </c>
-      <c r="I26" s="124" t="s">
-        <v>143</v>
-      </c>
-      <c r="J26" s="124" t="s">
-        <v>144</v>
-      </c>
-      <c r="K26" s="136" t="s">
-        <v>137</v>
-      </c>
-      <c r="L26" s="132" t="s">
-        <v>130</v>
-      </c>
-      <c r="M26" s="31"/>
-      <c r="N26" s="133" t="s">
-        <v>145</v>
+      <c r="G26" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="H26" s="30"/>
+      <c r="I26" s="62" t="s">
+        <v>140</v>
+      </c>
+      <c r="J26" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="K26" s="30"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="56" t="s">
+        <v>142</v>
       </c>
       <c r="O26" s="99"/>
     </row>
@@ -4613,19 +4721,33 @@
         <v>11</v>
       </c>
       <c r="C27" s="45"/>
-      <c r="D27" s="130"/>
+      <c r="D27" s="144" t="s">
+        <v>165</v>
+      </c>
       <c r="E27" s="11" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="F27" s="35"/>
-      <c r="G27" s="135"/>
-      <c r="H27" s="136"/>
-      <c r="I27" s="125"/>
-      <c r="J27" s="125"/>
-      <c r="K27" s="136"/>
-      <c r="L27" s="132"/>
+      <c r="G27" s="149"/>
+      <c r="H27" s="150" t="s">
+        <v>128</v>
+      </c>
+      <c r="I27" s="138" t="s">
+        <v>143</v>
+      </c>
+      <c r="J27" s="138" t="s">
+        <v>144</v>
+      </c>
+      <c r="K27" s="150" t="s">
+        <v>137</v>
+      </c>
+      <c r="L27" s="146" t="s">
+        <v>130</v>
+      </c>
       <c r="M27" s="31"/>
-      <c r="N27" s="134"/>
+      <c r="N27" s="147" t="s">
+        <v>145</v>
+      </c>
       <c r="O27" s="99"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.65">
@@ -4636,21 +4758,19 @@
         <v>11</v>
       </c>
       <c r="C28" s="45"/>
-      <c r="D28" s="130" t="s">
-        <v>167</v>
-      </c>
+      <c r="D28" s="144"/>
       <c r="E28" s="11" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="F28" s="35"/>
-      <c r="G28" s="135"/>
-      <c r="H28" s="136"/>
-      <c r="I28" s="125"/>
-      <c r="J28" s="125"/>
-      <c r="K28" s="136"/>
-      <c r="L28" s="132"/>
+      <c r="G28" s="149"/>
+      <c r="H28" s="150"/>
+      <c r="I28" s="139"/>
+      <c r="J28" s="139"/>
+      <c r="K28" s="150"/>
+      <c r="L28" s="146"/>
       <c r="M28" s="31"/>
-      <c r="N28" s="134"/>
+      <c r="N28" s="148"/>
       <c r="O28" s="99"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.65">
@@ -4661,19 +4781,21 @@
         <v>11</v>
       </c>
       <c r="C29" s="45"/>
-      <c r="D29" s="130"/>
+      <c r="D29" s="144" t="s">
+        <v>165</v>
+      </c>
       <c r="E29" s="11" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="F29" s="35"/>
-      <c r="G29" s="135"/>
-      <c r="H29" s="136"/>
-      <c r="I29" s="125"/>
-      <c r="J29" s="125"/>
-      <c r="K29" s="136"/>
-      <c r="L29" s="132"/>
+      <c r="G29" s="149"/>
+      <c r="H29" s="150"/>
+      <c r="I29" s="139"/>
+      <c r="J29" s="139"/>
+      <c r="K29" s="150"/>
+      <c r="L29" s="146"/>
       <c r="M29" s="31"/>
-      <c r="N29" s="134"/>
+      <c r="N29" s="148"/>
       <c r="O29" s="99"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.65">
@@ -4684,21 +4806,19 @@
         <v>11</v>
       </c>
       <c r="C30" s="45"/>
-      <c r="D30" s="130" t="s">
-        <v>167</v>
-      </c>
+      <c r="D30" s="144"/>
       <c r="E30" s="11" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="F30" s="35"/>
-      <c r="G30" s="135"/>
-      <c r="H30" s="136"/>
-      <c r="I30" s="125"/>
-      <c r="J30" s="125"/>
-      <c r="K30" s="136"/>
-      <c r="L30" s="132"/>
+      <c r="G30" s="149"/>
+      <c r="H30" s="150"/>
+      <c r="I30" s="139"/>
+      <c r="J30" s="139"/>
+      <c r="K30" s="150"/>
+      <c r="L30" s="146"/>
       <c r="M30" s="31"/>
-      <c r="N30" s="134"/>
+      <c r="N30" s="148"/>
       <c r="O30" s="99"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.65">
@@ -4709,19 +4829,21 @@
         <v>11</v>
       </c>
       <c r="C31" s="45"/>
-      <c r="D31" s="130"/>
+      <c r="D31" s="144" t="s">
+        <v>165</v>
+      </c>
       <c r="E31" s="11" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="F31" s="35"/>
-      <c r="G31" s="135"/>
-      <c r="H31" s="136"/>
-      <c r="I31" s="126"/>
-      <c r="J31" s="126"/>
-      <c r="K31" s="136"/>
-      <c r="L31" s="132"/>
+      <c r="G31" s="149"/>
+      <c r="H31" s="150"/>
+      <c r="I31" s="139"/>
+      <c r="J31" s="139"/>
+      <c r="K31" s="150"/>
+      <c r="L31" s="146"/>
       <c r="M31" s="31"/>
-      <c r="N31" s="134"/>
+      <c r="N31" s="148"/>
       <c r="O31" s="99"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.65">
@@ -4732,25 +4854,19 @@
         <v>11</v>
       </c>
       <c r="C32" s="45"/>
-      <c r="D32" s="130" t="s">
-        <v>167</v>
-      </c>
+      <c r="D32" s="144"/>
       <c r="E32" s="11" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="F32" s="35"/>
-      <c r="G32" s="135"/>
-      <c r="H32" s="136"/>
-      <c r="I32" s="124" t="s">
-        <v>146</v>
-      </c>
-      <c r="J32" s="124" t="s">
-        <v>147</v>
-      </c>
-      <c r="K32" s="136"/>
-      <c r="L32" s="132"/>
+      <c r="G32" s="149"/>
+      <c r="H32" s="150"/>
+      <c r="I32" s="140"/>
+      <c r="J32" s="140"/>
+      <c r="K32" s="150"/>
+      <c r="L32" s="146"/>
       <c r="M32" s="31"/>
-      <c r="N32" s="134"/>
+      <c r="N32" s="148"/>
       <c r="O32" s="99"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.65">
@@ -4761,19 +4877,25 @@
         <v>11</v>
       </c>
       <c r="C33" s="45"/>
-      <c r="D33" s="130"/>
+      <c r="D33" s="144" t="s">
+        <v>165</v>
+      </c>
       <c r="E33" s="11" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="F33" s="35"/>
-      <c r="G33" s="135"/>
-      <c r="H33" s="136"/>
-      <c r="I33" s="125"/>
-      <c r="J33" s="125"/>
-      <c r="K33" s="136"/>
-      <c r="L33" s="132"/>
+      <c r="G33" s="149"/>
+      <c r="H33" s="150"/>
+      <c r="I33" s="138" t="s">
+        <v>146</v>
+      </c>
+      <c r="J33" s="138" t="s">
+        <v>147</v>
+      </c>
+      <c r="K33" s="150"/>
+      <c r="L33" s="146"/>
       <c r="M33" s="31"/>
-      <c r="N33" s="134"/>
+      <c r="N33" s="148"/>
       <c r="O33" s="99"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.65">
@@ -4784,21 +4906,19 @@
         <v>11</v>
       </c>
       <c r="C34" s="45"/>
-      <c r="D34" s="130" t="s">
-        <v>167</v>
-      </c>
+      <c r="D34" s="144"/>
       <c r="E34" s="11" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="F34" s="35"/>
-      <c r="G34" s="135"/>
-      <c r="H34" s="136"/>
-      <c r="I34" s="125"/>
-      <c r="J34" s="125"/>
-      <c r="K34" s="136"/>
-      <c r="L34" s="132"/>
+      <c r="G34" s="149"/>
+      <c r="H34" s="150"/>
+      <c r="I34" s="139"/>
+      <c r="J34" s="139"/>
+      <c r="K34" s="150"/>
+      <c r="L34" s="146"/>
       <c r="M34" s="31"/>
-      <c r="N34" s="134"/>
+      <c r="N34" s="148"/>
       <c r="O34" s="99"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.65">
@@ -4809,19 +4929,21 @@
         <v>11</v>
       </c>
       <c r="C35" s="45"/>
-      <c r="D35" s="130"/>
+      <c r="D35" s="144" t="s">
+        <v>165</v>
+      </c>
       <c r="E35" s="11" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="F35" s="35"/>
-      <c r="G35" s="135"/>
-      <c r="H35" s="136"/>
-      <c r="I35" s="125"/>
-      <c r="J35" s="125"/>
-      <c r="K35" s="136"/>
-      <c r="L35" s="132"/>
+      <c r="G35" s="149"/>
+      <c r="H35" s="150"/>
+      <c r="I35" s="139"/>
+      <c r="J35" s="139"/>
+      <c r="K35" s="150"/>
+      <c r="L35" s="146"/>
       <c r="M35" s="31"/>
-      <c r="N35" s="134"/>
+      <c r="N35" s="148"/>
       <c r="O35" s="99"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.65">
@@ -4832,21 +4954,19 @@
         <v>11</v>
       </c>
       <c r="C36" s="45"/>
-      <c r="D36" s="130" t="s">
-        <v>167</v>
-      </c>
+      <c r="D36" s="144"/>
       <c r="E36" s="11" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="F36" s="35"/>
-      <c r="G36" s="135"/>
-      <c r="H36" s="136"/>
-      <c r="I36" s="125"/>
-      <c r="J36" s="125"/>
-      <c r="K36" s="136"/>
-      <c r="L36" s="132"/>
+      <c r="G36" s="149"/>
+      <c r="H36" s="150"/>
+      <c r="I36" s="139"/>
+      <c r="J36" s="139"/>
+      <c r="K36" s="150"/>
+      <c r="L36" s="146"/>
       <c r="M36" s="31"/>
-      <c r="N36" s="134"/>
+      <c r="N36" s="148"/>
       <c r="O36" s="99"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.65">
@@ -4857,19 +4977,21 @@
         <v>11</v>
       </c>
       <c r="C37" s="45"/>
-      <c r="D37" s="130"/>
+      <c r="D37" s="144" t="s">
+        <v>165</v>
+      </c>
       <c r="E37" s="11" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="F37" s="35"/>
-      <c r="G37" s="135"/>
-      <c r="H37" s="136"/>
-      <c r="I37" s="126"/>
-      <c r="J37" s="126"/>
-      <c r="K37" s="136"/>
-      <c r="L37" s="132"/>
+      <c r="G37" s="149"/>
+      <c r="H37" s="150"/>
+      <c r="I37" s="139"/>
+      <c r="J37" s="139"/>
+      <c r="K37" s="150"/>
+      <c r="L37" s="146"/>
       <c r="M37" s="31"/>
-      <c r="N37" s="134"/>
+      <c r="N37" s="148"/>
       <c r="O37" s="99"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.65">
@@ -4880,25 +5002,19 @@
         <v>11</v>
       </c>
       <c r="C38" s="45"/>
-      <c r="D38" s="130" t="s">
-        <v>167</v>
-      </c>
+      <c r="D38" s="144"/>
       <c r="E38" s="11" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="F38" s="35"/>
-      <c r="G38" s="135"/>
-      <c r="H38" s="136"/>
-      <c r="I38" s="124" t="s">
-        <v>166</v>
-      </c>
-      <c r="J38" s="127" t="s">
-        <v>148</v>
-      </c>
-      <c r="K38" s="136"/>
-      <c r="L38" s="132"/>
+      <c r="G38" s="149"/>
+      <c r="H38" s="150"/>
+      <c r="I38" s="140"/>
+      <c r="J38" s="140"/>
+      <c r="K38" s="150"/>
+      <c r="L38" s="146"/>
       <c r="M38" s="31"/>
-      <c r="N38" s="134"/>
+      <c r="N38" s="148"/>
       <c r="O38" s="99"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.65">
@@ -4909,19 +5025,25 @@
         <v>11</v>
       </c>
       <c r="C39" s="45"/>
-      <c r="D39" s="130"/>
+      <c r="D39" s="144" t="s">
+        <v>165</v>
+      </c>
       <c r="E39" s="11" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="F39" s="35"/>
-      <c r="G39" s="135"/>
-      <c r="H39" s="136"/>
-      <c r="I39" s="125"/>
-      <c r="J39" s="128"/>
-      <c r="K39" s="136"/>
-      <c r="L39" s="132"/>
+      <c r="G39" s="149"/>
+      <c r="H39" s="150"/>
+      <c r="I39" s="138" t="s">
+        <v>164</v>
+      </c>
+      <c r="J39" s="141" t="s">
+        <v>148</v>
+      </c>
+      <c r="K39" s="150"/>
+      <c r="L39" s="146"/>
       <c r="M39" s="31"/>
-      <c r="N39" s="134"/>
+      <c r="N39" s="148"/>
       <c r="O39" s="99"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.65">
@@ -4932,21 +5054,19 @@
         <v>11</v>
       </c>
       <c r="C40" s="45"/>
-      <c r="D40" s="130" t="s">
-        <v>167</v>
-      </c>
+      <c r="D40" s="144"/>
       <c r="E40" s="11" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="F40" s="35"/>
-      <c r="G40" s="135"/>
-      <c r="H40" s="136"/>
-      <c r="I40" s="125"/>
-      <c r="J40" s="128"/>
-      <c r="K40" s="136"/>
-      <c r="L40" s="132"/>
+      <c r="G40" s="149"/>
+      <c r="H40" s="150"/>
+      <c r="I40" s="139"/>
+      <c r="J40" s="142"/>
+      <c r="K40" s="150"/>
+      <c r="L40" s="146"/>
       <c r="M40" s="31"/>
-      <c r="N40" s="134"/>
+      <c r="N40" s="148"/>
       <c r="O40" s="99"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.65">
@@ -4957,19 +5077,21 @@
         <v>11</v>
       </c>
       <c r="C41" s="45"/>
-      <c r="D41" s="130"/>
+      <c r="D41" s="144" t="s">
+        <v>165</v>
+      </c>
       <c r="E41" s="11" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="F41" s="35"/>
-      <c r="G41" s="135"/>
-      <c r="H41" s="136"/>
-      <c r="I41" s="125"/>
-      <c r="J41" s="128"/>
-      <c r="K41" s="136"/>
-      <c r="L41" s="132"/>
+      <c r="G41" s="149"/>
+      <c r="H41" s="150"/>
+      <c r="I41" s="139"/>
+      <c r="J41" s="142"/>
+      <c r="K41" s="150"/>
+      <c r="L41" s="146"/>
       <c r="M41" s="31"/>
-      <c r="N41" s="134"/>
+      <c r="N41" s="148"/>
       <c r="O41" s="99"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.65">
@@ -4977,26 +5099,22 @@
         <v>44352</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D42" s="130" t="s">
-        <v>167</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>72</v>
+        <v>11</v>
+      </c>
+      <c r="C42" s="45"/>
+      <c r="D42" s="144"/>
+      <c r="E42" s="11" t="s">
+        <v>101</v>
       </c>
       <c r="F42" s="35"/>
-      <c r="G42" s="135"/>
-      <c r="H42" s="136"/>
-      <c r="I42" s="125"/>
-      <c r="J42" s="128"/>
-      <c r="K42" s="136"/>
-      <c r="L42" s="132"/>
+      <c r="G42" s="149"/>
+      <c r="H42" s="150"/>
+      <c r="I42" s="139"/>
+      <c r="J42" s="142"/>
+      <c r="K42" s="150"/>
+      <c r="L42" s="146"/>
       <c r="M42" s="31"/>
-      <c r="N42" s="134"/>
+      <c r="N42" s="148"/>
       <c r="O42" s="99"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.65">
@@ -5006,114 +5124,116 @@
       <c r="B43" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="130"/>
-      <c r="E43" s="94"/>
+      <c r="C43" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="144" t="s">
+        <v>165</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>72</v>
+      </c>
       <c r="F43" s="35"/>
-      <c r="G43" s="135"/>
-      <c r="H43" s="136"/>
-      <c r="I43" s="126"/>
-      <c r="J43" s="129"/>
-      <c r="K43" s="136"/>
-      <c r="L43" s="132"/>
+      <c r="G43" s="149"/>
+      <c r="H43" s="150"/>
+      <c r="I43" s="139"/>
+      <c r="J43" s="142"/>
+      <c r="K43" s="150"/>
+      <c r="L43" s="146"/>
       <c r="M43" s="31"/>
-      <c r="N43" s="134"/>
+      <c r="N43" s="148"/>
       <c r="O43" s="99"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="A44" s="39"/>
-      <c r="B44" s="40"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="41"/>
+      <c r="A44" s="26">
+        <v>44352</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="4"/>
+      <c r="D44" s="144"/>
+      <c r="E44" s="94"/>
       <c r="F44" s="35"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="43"/>
-      <c r="K44" s="28"/>
-      <c r="L44" s="43"/>
-      <c r="M44" s="40"/>
-      <c r="N44" s="44"/>
+      <c r="G44" s="149"/>
+      <c r="H44" s="150"/>
+      <c r="I44" s="140"/>
+      <c r="J44" s="143"/>
+      <c r="K44" s="150"/>
+      <c r="L44" s="146"/>
+      <c r="M44" s="31"/>
+      <c r="N44" s="148"/>
       <c r="O44" s="99"/>
     </row>
-    <row r="45" spans="1:15" ht="132.30000000000001" x14ac:dyDescent="0.65">
-      <c r="A45" s="26">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.65">
+      <c r="A45" s="39"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="41"/>
+      <c r="E45" s="41"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="42"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="43"/>
+      <c r="K45" s="28"/>
+      <c r="L45" s="43"/>
+      <c r="M45" s="40"/>
+      <c r="N45" s="44"/>
+      <c r="O45" s="99"/>
+    </row>
+    <row r="46" spans="1:15" ht="132.30000000000001" x14ac:dyDescent="0.65">
+      <c r="A46" s="26">
         <v>44352</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="48" t="s">
+      <c r="C46" s="4"/>
+      <c r="D46" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E45" s="61" t="s">
-        <v>187</v>
-      </c>
-      <c r="F45" s="35"/>
-      <c r="G45" s="60"/>
-      <c r="H45" s="98" t="s">
+      <c r="E46" s="61" t="s">
+        <v>183</v>
+      </c>
+      <c r="F46" s="35"/>
+      <c r="G46" s="60"/>
+      <c r="H46" s="98" t="s">
         <v>128</v>
       </c>
-      <c r="I45" s="48" t="s">
+      <c r="I46" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="J45" s="31" t="s">
+      <c r="J46" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="K45" s="98" t="s">
+      <c r="K46" s="98" t="s">
         <v>115</v>
       </c>
-      <c r="L45" s="31" t="s">
+      <c r="L46" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="M45" s="31"/>
-      <c r="N45" s="56" t="s">
-        <v>198</v>
-      </c>
-      <c r="O45" s="99"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="A46" s="39"/>
-      <c r="B46" s="40"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="28"/>
-      <c r="I46" s="41"/>
-      <c r="J46" s="43"/>
-      <c r="K46" s="28"/>
-      <c r="L46" s="43"/>
-      <c r="M46" s="40"/>
-      <c r="N46" s="44"/>
+      <c r="M46" s="31"/>
+      <c r="N46" s="56" t="s">
+        <v>194</v>
+      </c>
       <c r="O46" s="99"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="A47" s="26">
-        <v>44352</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
+      <c r="A47" s="39"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
       <c r="F47" s="35"/>
-      <c r="G47" s="60" t="s">
-        <v>149</v>
-      </c>
-      <c r="H47" s="8"/>
-      <c r="I47" s="54"/>
-      <c r="J47" s="53"/>
-      <c r="K47" s="69"/>
-      <c r="L47" s="54"/>
-      <c r="M47" s="70"/>
-      <c r="N47" s="131" t="s">
-        <v>150</v>
-      </c>
+      <c r="G47" s="42"/>
+      <c r="H47" s="28"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="43"/>
+      <c r="K47" s="28"/>
+      <c r="L47" s="43"/>
+      <c r="M47" s="40"/>
+      <c r="N47" s="44"/>
       <c r="O47" s="99"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.65">
@@ -5124,21 +5244,21 @@
         <v>11</v>
       </c>
       <c r="C48" s="12"/>
-      <c r="D48" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>37</v>
-      </c>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
       <c r="F48" s="35"/>
-      <c r="G48" s="60"/>
-      <c r="H48" s="71"/>
-      <c r="I48" s="57"/>
-      <c r="J48" s="49"/>
-      <c r="K48" s="72"/>
-      <c r="L48" s="57"/>
-      <c r="M48" s="73"/>
-      <c r="N48" s="131"/>
+      <c r="G48" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="H48" s="8"/>
+      <c r="I48" s="54"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="69"/>
+      <c r="L48" s="54"/>
+      <c r="M48" s="70"/>
+      <c r="N48" s="145" t="s">
+        <v>150</v>
+      </c>
       <c r="O48" s="99"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.65">
@@ -5153,7 +5273,7 @@
         <v>12</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F49" s="35"/>
       <c r="G49" s="60"/>
@@ -5163,7 +5283,7 @@
       <c r="K49" s="72"/>
       <c r="L49" s="57"/>
       <c r="M49" s="73"/>
-      <c r="N49" s="131"/>
+      <c r="N49" s="145"/>
       <c r="O49" s="99"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.65">
@@ -5178,7 +5298,7 @@
         <v>12</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F50" s="35"/>
       <c r="G50" s="60"/>
@@ -5188,7 +5308,7 @@
       <c r="K50" s="72"/>
       <c r="L50" s="57"/>
       <c r="M50" s="73"/>
-      <c r="N50" s="131"/>
+      <c r="N50" s="145"/>
       <c r="O50" s="99"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.65">
@@ -5203,7 +5323,7 @@
         <v>12</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F51" s="35"/>
       <c r="G51" s="60"/>
@@ -5213,7 +5333,7 @@
       <c r="K51" s="72"/>
       <c r="L51" s="57"/>
       <c r="M51" s="73"/>
-      <c r="N51" s="131"/>
+      <c r="N51" s="145"/>
       <c r="O51" s="99"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.65">
@@ -5228,7 +5348,7 @@
         <v>12</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F52" s="35"/>
       <c r="G52" s="60"/>
@@ -5238,7 +5358,7 @@
       <c r="K52" s="72"/>
       <c r="L52" s="57"/>
       <c r="M52" s="73"/>
-      <c r="N52" s="131"/>
+      <c r="N52" s="145"/>
       <c r="O52" s="99"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.65">
@@ -5253,7 +5373,7 @@
         <v>12</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F53" s="35"/>
       <c r="G53" s="60"/>
@@ -5263,7 +5383,7 @@
       <c r="K53" s="72"/>
       <c r="L53" s="57"/>
       <c r="M53" s="73"/>
-      <c r="N53" s="131"/>
+      <c r="N53" s="145"/>
       <c r="O53" s="99"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.65">
@@ -5278,7 +5398,7 @@
         <v>12</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F54" s="35"/>
       <c r="G54" s="60"/>
@@ -5288,7 +5408,7 @@
       <c r="K54" s="72"/>
       <c r="L54" s="57"/>
       <c r="M54" s="73"/>
-      <c r="N54" s="131"/>
+      <c r="N54" s="145"/>
       <c r="O54" s="99"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.65">
@@ -5303,7 +5423,7 @@
         <v>12</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F55" s="35"/>
       <c r="G55" s="60"/>
@@ -5313,7 +5433,7 @@
       <c r="K55" s="72"/>
       <c r="L55" s="57"/>
       <c r="M55" s="73"/>
-      <c r="N55" s="131"/>
+      <c r="N55" s="145"/>
       <c r="O55" s="99"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.65">
@@ -5321,14 +5441,14 @@
         <v>44352</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="C56" s="12"/>
       <c r="D56" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E56" s="14" t="s">
-        <v>72</v>
+      <c r="E56" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="F56" s="35"/>
       <c r="G56" s="60"/>
@@ -5338,76 +5458,101 @@
       <c r="K56" s="72"/>
       <c r="L56" s="57"/>
       <c r="M56" s="73"/>
-      <c r="N56" s="131"/>
+      <c r="N56" s="145"/>
       <c r="O56" s="99"/>
     </row>
-    <row r="57" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A57" s="74"/>
-      <c r="B57" s="75"/>
-      <c r="C57" s="76"/>
-      <c r="D57" s="76"/>
-      <c r="E57" s="76"/>
-      <c r="F57" s="77"/>
-      <c r="G57" s="78"/>
-      <c r="H57" s="79"/>
-      <c r="I57" s="76"/>
-      <c r="J57" s="80"/>
-      <c r="K57" s="79"/>
-      <c r="L57" s="80"/>
-      <c r="M57" s="75"/>
-      <c r="N57" s="81"/>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.65">
+      <c r="A57" s="26">
+        <v>44352</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" s="12"/>
+      <c r="D57" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F57" s="35"/>
+      <c r="G57" s="60"/>
+      <c r="H57" s="71"/>
+      <c r="I57" s="57"/>
+      <c r="J57" s="49"/>
+      <c r="K57" s="72"/>
+      <c r="L57" s="57"/>
+      <c r="M57" s="73"/>
+      <c r="N57" s="145"/>
       <c r="O57" s="99"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="E59" s="110"/>
+    <row r="58" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A58" s="74"/>
+      <c r="B58" s="75"/>
+      <c r="C58" s="76"/>
+      <c r="D58" s="76"/>
+      <c r="E58" s="76"/>
+      <c r="F58" s="77"/>
+      <c r="G58" s="78"/>
+      <c r="H58" s="79"/>
+      <c r="I58" s="76"/>
+      <c r="J58" s="80"/>
+      <c r="K58" s="79"/>
+      <c r="L58" s="80"/>
+      <c r="M58" s="75"/>
+      <c r="N58" s="81"/>
+      <c r="O58" s="99"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.65">
       <c r="E60" s="110"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="E61" s="111"/>
+      <c r="E61" s="110"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.65">
       <c r="E62" s="111"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="E63" s="110"/>
+      <c r="E63" s="111"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.65">
       <c r="E64" s="110"/>
     </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.65">
+      <c r="E65" s="110"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N57" xr:uid="{E201601C-0217-4F72-B294-396D8744DE8C}"/>
+  <autoFilter ref="A1:N58" xr:uid="{E201601C-0217-4F72-B294-396D8744DE8C}"/>
   <mergeCells count="21">
-    <mergeCell ref="N47:N56"/>
-    <mergeCell ref="L26:L43"/>
-    <mergeCell ref="N26:N43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="I26:I31"/>
-    <mergeCell ref="J26:J31"/>
-    <mergeCell ref="I32:I37"/>
-    <mergeCell ref="J32:J37"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="G26:G43"/>
-    <mergeCell ref="H26:H43"/>
-    <mergeCell ref="K26:K43"/>
-    <mergeCell ref="I38:I43"/>
-    <mergeCell ref="J38:J43"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="N48:N57"/>
+    <mergeCell ref="L27:L44"/>
+    <mergeCell ref="N27:N44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="J27:J32"/>
+    <mergeCell ref="I33:I38"/>
+    <mergeCell ref="J33:J38"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="G27:G44"/>
+    <mergeCell ref="H27:H44"/>
+    <mergeCell ref="K27:K44"/>
+    <mergeCell ref="I39:I44"/>
+    <mergeCell ref="J39:J44"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D37:D38"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L13" r:id="rId1" location="SeqNum" xr:uid="{4596CCB4-330F-4F75-B9A0-3A04A4515CC6}"/>
-    <hyperlink ref="L17" r:id="rId2" xr:uid="{0837CCDD-84AD-4A47-B259-994CF7F15CAA}"/>
+    <hyperlink ref="L18" r:id="rId2" xr:uid="{0837CCDD-84AD-4A47-B259-994CF7F15CAA}"/>
     <hyperlink ref="M10" r:id="rId3" xr:uid="{FE3ED6D6-1069-41B9-8FD8-2CE7CBD2E4BA}"/>
     <hyperlink ref="M11" r:id="rId4" xr:uid="{50FE82B3-0275-4591-A185-179624E50F39}"/>
     <hyperlink ref="L15" r:id="rId5" location="statistical-article" xr:uid="{D33C6AAD-0534-4CAA-A08E-8877F510A350}"/>
-    <hyperlink ref="L18" r:id="rId6" location="eurostat" xr:uid="{594CC770-9DAC-442E-81AD-70565D583FEE}"/>
+    <hyperlink ref="L19" r:id="rId6" location="eurostat" xr:uid="{594CC770-9DAC-442E-81AD-70565D583FEE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -5428,10 +5573,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9EA5D7-1E13-41DC-A4C8-96CDED6C6F08}">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B18" sqref="A18:XFD18"/>
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.7" x14ac:dyDescent="0.65"/>
@@ -5716,7 +5861,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="27"/>
@@ -5729,8 +5874,8 @@
         <v>115</v>
       </c>
       <c r="L10" s="29"/>
-      <c r="M10" s="142" t="s">
-        <v>190</v>
+      <c r="M10" s="119" t="s">
+        <v>186</v>
       </c>
       <c r="N10" s="32"/>
       <c r="O10" s="100"/>
@@ -5743,7 +5888,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="45" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="34"/>
@@ -5756,8 +5901,8 @@
         <v>115</v>
       </c>
       <c r="L11" s="29"/>
-      <c r="M11" s="142" t="s">
-        <v>191</v>
+      <c r="M11" s="119" t="s">
+        <v>187</v>
       </c>
       <c r="N11" s="32"/>
       <c r="O11" s="99"/>
@@ -5781,14 +5926,16 @@
     </row>
     <row r="13" spans="1:15" ht="73.5" x14ac:dyDescent="0.65">
       <c r="A13" s="26">
-        <v>44399</v>
+        <v>44424</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="143" t="s">
-        <v>171</v>
+      <c r="C13" s="45" t="s">
+        <v>211</v>
+      </c>
+      <c r="D13" s="120" t="s">
+        <v>167</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="35"/>
@@ -5796,7 +5943,7 @@
         <v>127</v>
       </c>
       <c r="H13" s="48" t="s">
-        <v>169</v>
+        <v>209</v>
       </c>
       <c r="I13" s="57"/>
       <c r="J13" s="34"/>
@@ -5804,7 +5951,7 @@
         <v>115</v>
       </c>
       <c r="L13" s="38" t="s">
-        <v>170</v>
+        <v>210</v>
       </c>
       <c r="M13" s="31"/>
       <c r="N13" s="56" t="s">
@@ -5821,7 +5968,7 @@
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="35"/>
@@ -5841,7 +5988,7 @@
       <c r="L14" s="14"/>
       <c r="M14" s="103"/>
       <c r="N14" s="56" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="O14" s="99"/>
     </row>
@@ -5854,7 +6001,7 @@
       </c>
       <c r="C15" s="45"/>
       <c r="D15" s="48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E15" s="102" t="s">
         <v>80</v>
@@ -5874,11 +6021,11 @@
         <v>115</v>
       </c>
       <c r="L15" s="38" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="M15" s="38"/>
       <c r="N15" s="101" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="O15" s="99"/>
     </row>
@@ -5891,7 +6038,7 @@
       </c>
       <c r="C16" s="45"/>
       <c r="D16" s="48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>30</v>
@@ -5915,111 +6062,113 @@
       <c r="N16" s="32"/>
       <c r="O16" s="99"/>
     </row>
-    <row r="17" spans="1:15" ht="29.4" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:15" ht="58.8" x14ac:dyDescent="0.65">
       <c r="A17" s="26">
-        <v>44392</v>
+        <v>44424</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="45"/>
+      <c r="C17" s="45" t="s">
+        <v>203</v>
+      </c>
       <c r="D17" s="48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="35"/>
       <c r="G17" s="52"/>
-      <c r="H17" s="113" t="s">
+      <c r="H17" s="122" t="s">
         <v>128</v>
       </c>
       <c r="I17" s="54" t="s">
-        <v>179</v>
-      </c>
-      <c r="J17" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="K17" s="113" t="s">
+        <v>204</v>
+      </c>
+      <c r="J17" s="53" t="s">
+        <v>132</v>
+      </c>
+      <c r="K17" s="122" t="s">
         <v>115</v>
       </c>
-      <c r="L17" s="38" t="s">
-        <v>180</v>
+      <c r="L17" s="123" t="s">
+        <v>205</v>
       </c>
       <c r="M17" s="31"/>
-      <c r="N17" s="32"/>
+      <c r="N17" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="O17" s="99"/>
     </row>
     <row r="18" spans="1:15" ht="29.4" x14ac:dyDescent="0.65">
       <c r="A18" s="26">
-        <v>44399</v>
+        <v>44392</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="45"/>
       <c r="D18" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="E18" s="102" t="s">
-        <v>78</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="E18" s="27"/>
       <c r="F18" s="35"/>
       <c r="G18" s="52"/>
-      <c r="H18" s="98" t="s">
+      <c r="H18" s="112" t="s">
         <v>128</v>
       </c>
-      <c r="I18" s="55" t="s">
-        <v>133</v>
+      <c r="I18" s="54" t="s">
+        <v>175</v>
       </c>
       <c r="J18" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="K18" s="98" t="s">
+      <c r="K18" s="112" t="s">
         <v>115</v>
       </c>
       <c r="L18" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="M18" s="38"/>
-      <c r="N18" s="101" t="s">
-        <v>195</v>
-      </c>
-      <c r="O18" s="99"/>
-    </row>
-    <row r="19" spans="1:15" ht="44.1" x14ac:dyDescent="0.65">
+        <v>176</v>
+      </c>
+      <c r="M18" s="31"/>
+      <c r="N18" s="32"/>
+    </row>
+    <row r="19" spans="1:15" ht="29.4" x14ac:dyDescent="0.65">
       <c r="A19" s="26">
-        <v>44353</v>
+        <v>44399</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="45"/>
       <c r="D19" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="E19" s="31" t="s">
-        <v>138</v>
+        <v>167</v>
+      </c>
+      <c r="E19" s="102" t="s">
+        <v>78</v>
       </c>
       <c r="F19" s="35"/>
       <c r="G19" s="52"/>
       <c r="H19" s="98" t="s">
         <v>128</v>
       </c>
-      <c r="I19" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="J19" s="58" t="s">
-        <v>135</v>
+      <c r="I19" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="J19" s="31" t="s">
+        <v>130</v>
       </c>
       <c r="K19" s="98" t="s">
         <v>115</v>
       </c>
-      <c r="L19" s="58"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="56" t="s">
-        <v>175</v>
+      <c r="L19" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="M19" s="38"/>
+      <c r="N19" s="101" t="s">
+        <v>191</v>
       </c>
       <c r="O19" s="99"/>
     </row>
-    <row r="20" spans="1:15" ht="29.4" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:15" ht="44.1" x14ac:dyDescent="0.65">
       <c r="A20" s="26">
         <v>44353</v>
       </c>
@@ -6028,205 +6177,240 @@
       </c>
       <c r="C20" s="45"/>
       <c r="D20" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>31</v>
+        <v>167</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>138</v>
       </c>
       <c r="F20" s="35"/>
       <c r="G20" s="52"/>
       <c r="H20" s="98" t="s">
         <v>128</v>
       </c>
-      <c r="I20" s="54" t="s">
-        <v>136</v>
-      </c>
-      <c r="J20" s="59" t="s">
-        <v>130</v>
+      <c r="I20" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="J20" s="58" t="s">
+        <v>135</v>
       </c>
       <c r="K20" s="98" t="s">
         <v>115</v>
       </c>
-      <c r="L20" s="59"/>
+      <c r="L20" s="58"/>
       <c r="M20" s="31"/>
-      <c r="N20" s="32"/>
+      <c r="N20" s="56" t="s">
+        <v>171</v>
+      </c>
       <c r="O20" s="99"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="A21" s="39"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
+    <row r="21" spans="1:15" ht="29.4" x14ac:dyDescent="0.65">
+      <c r="A21" s="26">
+        <v>44353</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="45"/>
+      <c r="D21" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="F21" s="35"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="40"/>
-      <c r="N21" s="44"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="98" t="s">
+        <v>128</v>
+      </c>
+      <c r="I21" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="J21" s="59" t="s">
+        <v>130</v>
+      </c>
+      <c r="K21" s="98" t="s">
+        <v>115</v>
+      </c>
+      <c r="L21" s="59"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="32"/>
       <c r="O21" s="99"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="A22" s="26">
-        <v>44352</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="45"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="7"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
       <c r="F22" s="35"/>
-      <c r="G22" s="60" t="s">
-        <v>139</v>
-      </c>
-      <c r="H22" s="30"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="63"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="56"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="44"/>
       <c r="O22" s="99"/>
     </row>
-    <row r="23" spans="1:15" ht="44.1" x14ac:dyDescent="0.65">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.65">
       <c r="A23" s="26">
         <v>44352</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="45"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="H23" s="30"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="99"/>
+    </row>
+    <row r="24" spans="1:15" ht="44.1" x14ac:dyDescent="0.65">
+      <c r="A24" s="26">
+        <v>44426</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="45"/>
+      <c r="D24" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="E24" s="124" t="s">
+        <v>212</v>
+      </c>
+      <c r="F24" s="35"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="105" t="s">
+        <v>128</v>
+      </c>
+      <c r="I24" s="106" t="s">
+        <v>172</v>
+      </c>
+      <c r="J24" s="66" t="s">
+        <v>173</v>
+      </c>
+      <c r="K24" s="98" t="s">
+        <v>115</v>
+      </c>
+      <c r="L24" s="66" t="s">
+        <v>130</v>
+      </c>
+      <c r="M24" s="67"/>
+      <c r="N24" s="97" t="s">
+        <v>174</v>
+      </c>
+      <c r="O24" s="99"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.65">
+      <c r="A25" s="39"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="99"/>
+    </row>
+    <row r="26" spans="1:15" ht="44.1" x14ac:dyDescent="0.65">
+      <c r="A26" s="26">
+        <v>44399</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="D23" s="104" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="94"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="105" t="s">
+      <c r="C26" s="4"/>
+      <c r="D26" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="E26" s="61" t="s">
+        <v>183</v>
+      </c>
+      <c r="F26" s="35"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="98" t="s">
         <v>128</v>
       </c>
-      <c r="I23" s="106" t="s">
-        <v>176</v>
-      </c>
-      <c r="J23" s="66" t="s">
-        <v>177</v>
-      </c>
-      <c r="K23" s="98" t="s">
+      <c r="I26" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="J26" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="K26" s="98" t="s">
         <v>115</v>
       </c>
-      <c r="L23" s="66" t="s">
+      <c r="L26" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="M23" s="67"/>
-      <c r="N23" s="97" t="s">
-        <v>178</v>
-      </c>
-      <c r="O23" s="99"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="A24" s="39"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="44"/>
-      <c r="O24" s="99"/>
-    </row>
-    <row r="25" spans="1:15" ht="44.1" x14ac:dyDescent="0.65">
-      <c r="A25" s="26">
-        <v>44399</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="61" t="s">
-        <v>187</v>
-      </c>
-      <c r="F25" s="35"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="98" t="s">
-        <v>128</v>
-      </c>
-      <c r="I25" s="48" t="s">
-        <v>158</v>
-      </c>
-      <c r="J25" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="K25" s="98" t="s">
-        <v>115</v>
-      </c>
-      <c r="L25" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="M25" s="31"/>
-      <c r="N25" s="56" t="s">
-        <v>200</v>
-      </c>
-      <c r="O25" s="99"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="A26" s="39"/>
-      <c r="B26" s="40"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="40"/>
-      <c r="N26" s="44"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="56" t="s">
+        <v>196</v>
+      </c>
       <c r="O26" s="99"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="E28" s="110"/>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.65">
+      <c r="A27" s="39"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="40"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="99"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.65">
       <c r="E29" s="110"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="E30" s="111"/>
+      <c r="E30" s="110"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.65">
       <c r="E31" s="111"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="E32" s="110"/>
+      <c r="E32" s="111"/>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.65">
       <c r="E33" s="110"/>
     </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.65">
+      <c r="E34" s="110"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N26" xr:uid="{E201601C-0217-4F72-B294-396D8744DE8C}"/>
+  <autoFilter ref="A1:N27" xr:uid="{E201601C-0217-4F72-B294-396D8744DE8C}"/>
   <hyperlinks>
     <hyperlink ref="L13" r:id="rId1" location="SeqNum" xr:uid="{DC78C549-B21D-433B-A133-9BAEF049FE75}"/>
-    <hyperlink ref="L17" r:id="rId2" xr:uid="{7D0220E6-08FB-4E30-BF8A-A70FCDD0ACD2}"/>
+    <hyperlink ref="L18" r:id="rId2" xr:uid="{7D0220E6-08FB-4E30-BF8A-A70FCDD0ACD2}"/>
     <hyperlink ref="M10" r:id="rId3" xr:uid="{6916C690-787A-49BA-8DA8-C54D617A98D4}"/>
     <hyperlink ref="M11" r:id="rId4" xr:uid="{28E52552-5167-44A6-8A0E-6ADFF4210927}"/>
     <hyperlink ref="L15" r:id="rId5" location="statistics-explained-data " xr:uid="{F1FD0720-F625-4527-85A5-4C42D74AF8C1}"/>
-    <hyperlink ref="L18" r:id="rId6" location="eurostat" xr:uid="{910AA4D8-E521-469D-A951-68BB9F412FB4}"/>
+    <hyperlink ref="L19" r:id="rId6" location="eurostat" xr:uid="{910AA4D8-E521-469D-A951-68BB9F412FB4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>

</xml_diff>